<commit_message>
Replace incorrect file with correct one
</commit_message>
<xml_diff>
--- a/Manual task/High level test plan.xlsx
+++ b/Manual task/High level test plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7962e5456b8557a6/Рабочий стол/Technical tasks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7962e5456b8557a6/Рабочий стол/Technical tasks/Appcharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{3F773495-ABE5-4F24-863B-F9B522ED6AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24A37AF9-4CF2-4490-8D49-67BC0CB639A7}"/>
+  <xr:revisionPtr revIDLastSave="391" documentId="8_{3F773495-ABE5-4F24-863B-F9B522ED6AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AA7444B-2990-4FBD-A231-7AB71F94C2CF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{E92EBB03-34FF-478C-A379-73367406BC8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{E92EBB03-34FF-478C-A379-73367406BC8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
-  <si>
-    <t>Online Banking Application</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>Prepared by Lusine Sargsyan</t>
   </si>
@@ -152,9 +149,6 @@
     <t>Further testing is out of budget</t>
   </si>
   <si>
-    <t>No high risk features/areas are left without testing (login/authorization, core banking features)</t>
-  </si>
-  <si>
     <t>2. Non-functional testing  including:</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
   </si>
   <si>
     <t>Load testing</t>
-  </si>
-  <si>
-    <t>Usability testing</t>
   </si>
   <si>
     <t>Test design techniques to be used</t>
@@ -189,24 +180,6 @@
     <t>5. Error Guessing</t>
   </si>
   <si>
-    <t>Test scenarios</t>
-  </si>
-  <si>
-    <t>2. Funds transfer</t>
-  </si>
-  <si>
-    <t>4. Transacion history</t>
-  </si>
-  <si>
-    <t>3. Bills/Payments</t>
-  </si>
-  <si>
-    <t>5. High traffic handling</t>
-  </si>
-  <si>
-    <t>6. Security checks</t>
-  </si>
-  <si>
     <t>Bug reporting</t>
   </si>
   <si>
@@ -225,78 +198,33 @@
     <t>5. Regression testing</t>
   </si>
   <si>
-    <t>6. Smoke and/or sanity testing.</t>
-  </si>
-  <si>
-    <t>7. Cross-browser and cross-platform testing.</t>
-  </si>
-  <si>
     <t>8. Acceptance testing</t>
   </si>
   <si>
-    <t>1. Functional testing - 4 weeks</t>
-  </si>
-  <si>
-    <t>2. Cross-browser and cross-platform testing - 1 week</t>
-  </si>
-  <si>
     <t>2.  Out of scope:</t>
   </si>
   <si>
     <t>4. Environments</t>
   </si>
   <si>
-    <t>3. Performance/load tests - 1 week</t>
-  </si>
-  <si>
     <t>Security testing</t>
   </si>
   <si>
-    <t>4. Security testing - 1 week</t>
-  </si>
-  <si>
-    <t>5. Usability testing - 1week</t>
-  </si>
-  <si>
-    <t>6. Regression testing - 1 week</t>
-  </si>
-  <si>
-    <t>7. Smoke and/or sanity testing -3 days</t>
-  </si>
-  <si>
-    <t>8. Acceptance testing - 3 days</t>
-  </si>
-  <si>
     <t>8. Roles and responsibilities</t>
   </si>
   <si>
     <t xml:space="preserve">Test schedule </t>
   </si>
   <si>
-    <t>The customer wants an online banking application supporting both desktop and mobile browsers. The application allows users to manage their bank accounts, transfer funds, pay bills, and view their transaction history.  This Test Plan document describes the appropriate strategies, processes, workflows, and methodologies used to plan, organize, execute and manage testing of the software project.</t>
-  </si>
-  <si>
-    <t>1. The main purpose of the test plan is to ensure that the system meets the requirements  (functional and non-functional): it means to validate the functionality, security, performance and compatibility of the online banking application.</t>
-  </si>
-  <si>
     <t>All  changes (including additions and deletions) to the requirements document, functional specification,design specification and so on will be  documented and tested at the highest level of quality allowed within the remaining time of the project and within the ability of the test team.</t>
   </si>
   <si>
-    <t>2. The second objective is to find out and expose all issues and risks, assign them to appropriate (responsible) team members , communicate with project team, ensure taht all issues are reviewed and/or fixed before release. To fulfill it, detailed testing is required, using different test methods and properly reporting all the defects.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Accessibility testing </t>
   </si>
   <si>
     <t>Third-part integration from backend side.</t>
   </si>
   <si>
-    <t>Writing and running automation scripts ( this is not covered by this test plan).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
     <r>
       <rPr>
         <i/>
@@ -306,18 +234,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Cross browser compatibility testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- that means to check how the application works on different platforms, the UI and the functionality on both desktop and mobile browsers on different operating systems.</t>
-    </r>
+      <t>Security testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - that means to check if the login and authentication process is secure and whether it is protected from unauthorized access or not. It's a high priority check.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Testing (testing purposes, including security and performance testing) </t>
+  </si>
+  <si>
+    <t>4. Production (the live environment )</t>
+  </si>
+  <si>
+    <t>Android  (different versions of android from oldest to be supported to latest)</t>
+  </si>
+  <si>
+    <t>macOS</t>
+  </si>
+  <si>
+    <t>Mobile devices, including iPhones and Android phones from different generations and different brands for Android phones (most common used devices in the regions which the application is supporting)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All the necessary documentation are ready and available </t>
+  </si>
+  <si>
+    <t>1. Functional testing - to validate that all the required features functioning properly.</t>
+  </si>
+  <si>
+    <t>1. Login and Authorization</t>
   </si>
   <si>
     <r>
@@ -329,17 +281,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Security testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - that means to check if the login and authentication process is secure and whether it is protected from unauthorized access or not. It's a high priority check.</t>
+      <t>Test manager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - responsible for communication coordination between team members and test progress reporting</t>
     </r>
   </si>
   <si>
@@ -352,6 +305,168 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">QA Lead </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-responsible for test environments, test case creating and execution, test progress monitoring</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>QA Engineer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - responsible for design, development and execution of test cases, test planning partisipation, bug reporting</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Performance tester </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- responsible for performance/load testing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Business Analyst</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - responsible for proper requirements</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Security tester</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - a security specialist,either outsourced or within the company, responsible for security testing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Product Owner or other stakeholders</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - responsible for providing feedback on test coverage, schedule and priorities  and approving readinnes to release </t>
+    </r>
+  </si>
+  <si>
+    <t>1. In Scope:</t>
+  </si>
+  <si>
+    <t>Tablets, including iPads and Android tabs from different generations and  different brands for Android tabs  (most common used devices in the regions which the application is supporting)</t>
+  </si>
+  <si>
+    <t>Appcharge</t>
+  </si>
+  <si>
+    <t>The stakeholders wants ensure that the platform allows users to add virtual goods to their store through a dashboard and sell the virtual goods to customers through the store. Appcharge is providing mobile gaming studios with a white-label web store solution to sell their virtual game goods outside of the game directly to their players with reduced fees.  This Test Plan document describes the appropriate strategies, processes, workflows, and methodologies used to plan, organize, execute and manage testing of the software project.</t>
+  </si>
+  <si>
+    <t>2. The second objective is to find out and expose all issues and risks, assign them to appropriate (responsible) team members , communicate with project team, ensure that all issues are reviewed and/or fixed before release. To fulfill it, detailed testing is required, using different test methods and properly reporting all the defects.</t>
+  </si>
+  <si>
+    <t>1. The main purpose of the test plan is to ensure that the system meets the requirements  (functional and non-functional): it means to validate the functionality, security and performance  of the application.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Features testing</t>
     </r>
     <r>
@@ -362,7 +477,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - all the features described in requirements (transfer funds between accounts, pay bills, and view transaction history) should work properly and without unexpected failures.</t>
+      <t xml:space="preserve"> - all the features described in requirements (adding virtual goods to their store through a dashboard and sell the virtual goods to customers through the store) should work properly and without unexpected failures.</t>
     </r>
   </si>
   <si>
@@ -385,7 +500,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- it is needed to validate that the application works without failures and loading issues under high traffic during peak hours.</t>
+      <t>- it is needed to validate that the application works without failures and loading issues under high traffic.</t>
     </r>
   </si>
   <si>
@@ -398,42 +513,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Compliance testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- checking if the data is protected via security checks to validate it meets industry-standard security practices.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Testing (testing purposes, including security and performance testing) </t>
-  </si>
-  <si>
-    <t>4. Production (the live environment )</t>
-  </si>
-  <si>
-    <t>Android  (different versions of android from oldest to be supported to latest)</t>
-  </si>
-  <si>
-    <t>macOS</t>
-  </si>
-  <si>
-    <t>Mobile devices, including iPhones and Android phones from different generations and different brands for Android phones (most common used devices in the regions which the application is supporting)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All the necessary documentation are ready and available </t>
-  </si>
-  <si>
-    <t>1. Functional testing - to validate that all the required features functioning properly.</t>
-  </si>
-  <si>
-    <t>1. Login and Authorization</t>
+      <t>Security compliance testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- checking if the data is protected via security checks to validate it meets industry-standard security practices and can handle .</t>
+    </r>
+  </si>
+  <si>
+    <t>No high risk features/areas are left without testing (login/authorization security, payment security, creating/selling products, performance)</t>
   </si>
   <si>
     <r>
@@ -445,7 +539,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test manager</t>
+      <t>Developers</t>
     </r>
     <r>
       <rPr>
@@ -456,185 +550,203 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - responsible for communication coordination between team members and test progress reporting</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">QA Lead </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-responsible for test environments, test case creating and execution, test progress monitoring</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>QA Engineer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - responsible for design, development and execution of test cases, test planning partisipation, bug reporting</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Performance tester </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- responsible for performance/load testing</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - responsible for debugging in providing information to QA Engineers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Business Analyst</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - responsible for proper requirements</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Security tester</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - a security specialist,either outsourced or within the company, responsible for security testing</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Product Owner or other stakeholders</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - responsible for providing feedback on test coverage, schedule and priorities  and approving readinnes to release </t>
-    </r>
-  </si>
-  <si>
-    <t>1. In Scope:</t>
-  </si>
-  <si>
-    <t>(for security testing security specialist should fill the tool)</t>
-  </si>
-  <si>
-    <t>Tablets, including iPads and Android tabs from different generations and  different brands for Android tabs  (most common used devices in the regions which the application is supporting)</t>
+      <t xml:space="preserve"> - responsible for debugging and providing information to QA Engineers</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Functional testing - 2 weeks</t>
+  </si>
+  <si>
+    <t>2. Performance/load tests - 1 week</t>
+  </si>
+  <si>
+    <t>3. Security testing - 1 week</t>
+  </si>
+  <si>
+    <t>Automate test cases</t>
+  </si>
+  <si>
+    <t>4. Test cases automation - 1 week</t>
+  </si>
+  <si>
+    <t>5. Regression testing - 1 week</t>
+  </si>
+  <si>
+    <t>6. Smoke and/or sanity testing -3 days</t>
+  </si>
+  <si>
+    <t>7. Acceptance testing - 3 days</t>
+  </si>
+  <si>
+    <t>2. Creating virtual products via dashboard</t>
+  </si>
+  <si>
+    <t>4. High traffic handling</t>
+  </si>
+  <si>
+    <t>5. Security checks</t>
+  </si>
+  <si>
+    <t>1.1. Check users can successfully login dashboard with valid data via username and password</t>
+  </si>
+  <si>
+    <t>1.2. Check users can't successfully login dashboard with invalid data via username and password</t>
+  </si>
+  <si>
+    <t>Test scenarios/Check list(samples)</t>
+  </si>
+  <si>
+    <t>3.2. Check if the customer can choose a product.</t>
+  </si>
+  <si>
+    <t>3.4. Check if the customer can pay for the good via credit card.</t>
+  </si>
+  <si>
+    <t>3.5. Check if the customer can pay for the good via PayPal.</t>
+  </si>
+  <si>
+    <t>3.6. Check if the customer can pay for the good via Link.</t>
+  </si>
+  <si>
+    <t>3.7. Check if the customer can pay for the good via Google Pay.</t>
+  </si>
+  <si>
+    <t>3.11. Check that the purchased item is displayed in Orders.</t>
+  </si>
+  <si>
+    <t>Stress testing</t>
+  </si>
+  <si>
+    <t>4.1. Check that the app behaves as required under high traffic simulation on the web store.</t>
+  </si>
+  <si>
+    <t>Web Dev tools</t>
+  </si>
+  <si>
+    <t>4.4.  Check that the store performes as usual  when load increases gradually.</t>
+  </si>
+  <si>
+    <t>4.5. Check that the store remains stable after a sudden load increase.</t>
+  </si>
+  <si>
+    <t>5.1. Check access control management</t>
+  </si>
+  <si>
+    <t>5.2. Penetration testing</t>
+  </si>
+  <si>
+    <t>5.5. Check session expiration</t>
+  </si>
+  <si>
+    <t>Security testing tools should be added by security specialist</t>
+  </si>
+  <si>
+    <t>1.3. Check the "Forget password" button functioning properly</t>
+  </si>
+  <si>
+    <t>1.4. Check the "Reveal password ('eye' icon)" button functioning properly</t>
+  </si>
+  <si>
+    <t>1.5. Check if users can successfully log in to the dashbord via "Google login" with valid data</t>
+  </si>
+  <si>
+    <t>1.6. Check if users can't log in to the dashbord via "Google login" with invalid data</t>
+  </si>
+  <si>
+    <t>2.1. Check that the user has access to the "Products" subsection from the "Studio" section.</t>
+  </si>
+  <si>
+    <t>2.2. Check the "Add New Product" button's functionality</t>
+  </si>
+  <si>
+    <t>2.3. Check that the fileds in "New Product" page can be filled as required.</t>
+  </si>
+  <si>
+    <t>2.4. Try  to save product with only the required fileds filled in.</t>
+  </si>
+  <si>
+    <t>2.5. Try to save product with each required field not filled in.</t>
+  </si>
+  <si>
+    <t>2.6. Save the product with all fields filled in.</t>
+  </si>
+  <si>
+    <t>2.7. Check the "Upload" functionality.</t>
+  </si>
+  <si>
+    <t>2.8. Check Edit/Duplicate/Delete functionalities.</t>
+  </si>
+  <si>
+    <t>2.9. Check the "Update Product" functionality.</t>
+  </si>
+  <si>
+    <t>2.10. Check that the user has access to the "Bundles" subsection in the "Offers" section.</t>
+  </si>
+  <si>
+    <t>2.11. Check the "Add New Bundle" button's functionality.</t>
+  </si>
+  <si>
+    <t>2.12. Check that the fields in "Add New Bundle" can be filled as required.</t>
+  </si>
+  <si>
+    <t>2.13. Try to save the bundle with only the required fields filled in.</t>
+  </si>
+  <si>
+    <t>2.14. Try to save the bundle with each required field not filled in.</t>
+  </si>
+  <si>
+    <t>2.15. Save the bundle with all fields filled in.</t>
+  </si>
+  <si>
+    <t>2.16. Check the "Add Product" button on the "New Bundle" page.</t>
+  </si>
+  <si>
+    <t>2.17. Check the design preview section while filling in the fields.</t>
+  </si>
+  <si>
+    <t>2.18. Check Edit/Duplicate/Delete functionalities.</t>
+  </si>
+  <si>
+    <t>2.19. Check that the product is displayed in the store.</t>
+  </si>
+  <si>
+    <t>3. Selling Virtual Goods to customers via Store</t>
+  </si>
+  <si>
+    <t>3.1. Check if the customer can log in to the store.</t>
+  </si>
+  <si>
+    <t>3.3. Check if the customer can be successfully navigated to the payment page.</t>
+  </si>
+  <si>
+    <t>3.8. Check that the customer can't buy the good with invalid data.</t>
+  </si>
+  <si>
+    <t>3.9. Check that the customer can't process the payment via card if not all required fields are filled in.</t>
+  </si>
+  <si>
+    <t>3.10. Check that all the details are properly displayed in the checkout details.</t>
+  </si>
+  <si>
+    <t>4.2. Check the breaking point of the system.</t>
+  </si>
+  <si>
+    <t>4.3. Check if the response remains stable during load testing.</t>
+  </si>
+  <si>
+    <t>5.6. Test for brute force attack</t>
+  </si>
+  <si>
+    <t>5.7. Test for URL manipulation</t>
+  </si>
+  <si>
+    <t>5.4. Check entry points</t>
+  </si>
+  <si>
+    <t>5.3. Check server access controls</t>
+  </si>
+  <si>
+    <t>6. Smoke or sanity testing.</t>
   </si>
 </sst>
 </file>
@@ -719,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -738,6 +850,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,7 +1192,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,7 +1202,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1097,12 +1210,12 @@
     </row>
     <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <v>45522</v>
+        <v>45526</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1110,52 +1223,52 @@
     </row>
     <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1165,66 +1278,60 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1A00F0-841B-468D-AF67-87D914A058B1}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1235,18 +1342,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3261FFDC-0C88-44B0-80D6-2D275D5D2EF2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="127.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1258,9 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A2D701-B184-44F8-B3D3-4FB9C8FC376D}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1269,12 +1372,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1282,7 +1385,7 @@
     </row>
     <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1292,40 +1395,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310FAAFF-7352-4541-BF8F-C8027538C45F}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="A2" s="8"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1333,22 +1436,17 @@
     </row>
     <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1368,27 +1466,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1398,32 +1496,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FAAA34A-4B3D-49C2-AED8-B835E935CB37}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1431,22 +1529,22 @@
     </row>
     <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1454,32 +1552,32 @@
     </row>
     <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1487,21 +1585,26 @@
     </row>
     <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1513,39 +1616,39 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1556,32 +1659,32 @@
     </row>
     <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1591,202 +1694,484 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23F74E9-2E3B-4611-B925-7696D61AAEA3}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
+      <c r="A13" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
+      <c r="B34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
+      <c r="B37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="8"/>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
+      <c r="B42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="8"/>
+      <c r="B43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="8"/>
+      <c r="B44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="8"/>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="8"/>
+      <c r="B46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="8"/>
+      <c r="B49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8"/>
+      <c r="B50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="8"/>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="8"/>
+      <c r="B52" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8"/>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8"/>
+      <c r="B54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8"/>
+      <c r="B55" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="8"/>
+      <c r="B56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="8"/>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="8"/>
+      <c r="B58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="8"/>
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+      <c r="B79" s="3"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1805,42 +2190,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>